<commit_message>
started with coursePlanning Patch
</commit_message>
<xml_diff>
--- a/storage/app/Testingdata/Tab2_Studienjahrgang.xlsx
+++ b/storage/app/Testingdata/Tab2_Studienjahrgang.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\mst\storage\app\Testingdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://supsign.sharepoint.com/sites/Intern/Freigegebene Dokumente/General/Kundendaten/HLS/Daten Evento/Export Juli 21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564A93AB-DF5A-4D09-A0A9-63658E37F965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{64EECA0F-D973-43B1-A267-E68259FA3244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05A30BAD-D689-4BF0-9D6B-7D23BEA84729}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$E$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$E$22</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>ID Anlass</t>
   </si>
@@ -34,6 +34,27 @@
     <t>Anlassbezeichnung</t>
   </si>
   <si>
+    <t>2-L-B-LSBZ/18.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Bioanalytik und Zellbiologie 2018</t>
+  </si>
+  <si>
+    <t>2-L-B-LSBZ/19</t>
+  </si>
+  <si>
+    <t>2-L-B-LSBZ/19.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Bioanalytik und Zellbiologie 2019</t>
+  </si>
+  <si>
+    <t>2-L-B-LSBZ/20.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Bioanalytik und Zellbiologie 2020</t>
+  </si>
+  <si>
     <t>2-L-B-LSCB/18.a-SJ</t>
   </si>
   <si>
@@ -41,6 +62,123 @@
   </si>
   <si>
     <t>2-L-B-LSCB/19</t>
+  </si>
+  <si>
+    <t>2-L-B-LSCB/19.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Chemie- und Bioprozesstechnik 2019</t>
+  </si>
+  <si>
+    <t>2-L-B-LSCB/20.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Chemie- und Bioprozesstechnik 2020</t>
+  </si>
+  <si>
+    <t>2-L-B-LSCH/18.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Chemie 2018</t>
+  </si>
+  <si>
+    <t>2-L-B-LSCH/19</t>
+  </si>
+  <si>
+    <t>2-L-B-LSCH/19.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Chemie 2019</t>
+  </si>
+  <si>
+    <t>2-L-B-LSCH/20.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Chemie 2020</t>
+  </si>
+  <si>
+    <t>2-L-B-LSMI/18.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Medizininformatik 2018</t>
+  </si>
+  <si>
+    <t>2-L-B-LSMI/19</t>
+  </si>
+  <si>
+    <t>2-L-B-LSMI/19.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Medizininformatik 2019</t>
+  </si>
+  <si>
+    <t>2-L-B-LSMI/20.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Medizininformatik 2020</t>
+  </si>
+  <si>
+    <t>2-L-B-LSMT/18.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Medizintechnik 2018</t>
+  </si>
+  <si>
+    <t>2-L-B-LSMT/19</t>
+  </si>
+  <si>
+    <t>2-L-B-LSMT/19.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Medizintechnik 2019</t>
+  </si>
+  <si>
+    <t>2-L-B-LSMT/20.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Medizintechnik 2020</t>
+  </si>
+  <si>
+    <t>2-L-B-LSPT/18.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Pharmatechnologie 2018</t>
+  </si>
+  <si>
+    <t>2-L-B-LSPT/19</t>
+  </si>
+  <si>
+    <t>2-L-B-LSPT/19.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Pharmatechnologie 2019</t>
+  </si>
+  <si>
+    <t>2-L-B-LSPT/20.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Pharmatechnologie 2020</t>
+  </si>
+  <si>
+    <t>2-L-B-LSUT/18.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Umwelttechnik 2018</t>
+  </si>
+  <si>
+    <t>2-L-B-LSUT/19</t>
+  </si>
+  <si>
+    <t>2-L-B-LSUT/19.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Umwelttechnik 2019</t>
+  </si>
+  <si>
+    <t>2-L-B-LSUT/20.a-SJ</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Life Sciences Umwelttechnik 2020</t>
   </si>
   <si>
     <t>Anlassnummer Stdg</t>
@@ -421,11 +559,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -448,15 +586,15 @@
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>1252215</v>
+        <v>9322951</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -465,41 +603,381 @@
         <v>4</v>
       </c>
       <c r="D2" s="10">
-        <v>9311288</v>
+        <v>9311263</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="4"/>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>9311732</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="10">
+        <v>9311263</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>9369191</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="10">
+        <v>9311263</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>9322952</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="10">
+        <v>9311288</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>9311734</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="10">
+        <v>9311288</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>9369194</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="10">
+        <v>9311288</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>9322953</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="10">
+        <v>9311212</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>9311735</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="10">
+        <v>9311212</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>9369195</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="10">
+        <v>9311212</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>9322955</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="10">
+        <v>9304956</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>9311737</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="10">
+        <v>9304956</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>9369197</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="10">
+        <v>9304956</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>9322956</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="10">
+        <v>9309072</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>9311738</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="10">
+        <v>9309072</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>9369169</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="10">
+        <v>9309072</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>9322957</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="10">
+        <v>9311111</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>9311739</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="10">
+        <v>9311111</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>9369199</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="10">
+        <v>9311111</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>9322950</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="10">
+        <v>9310716</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>9311740</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="10">
+        <v>9310716</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>9369200</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="10">
+        <v>9310716</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E22" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B2:E2 A3:E3 A1:C1" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:E19 A20:E23 A1:C1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -726,14 +1204,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B06904-67F3-400D-AB9B-3CD95CFC6F8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{359E82F3-A0BC-465A-8D41-7F73D23B566B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -742,21 +1212,14 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAA9CBFF-F379-4D9B-B674-AAE60B1F3E58}">
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B06904-67F3-400D-AB9B-3CD95CFC6F8C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fe8860e2-d6d8-4fb7-85c1-e3d670e00570"/>
-    <ds:schemaRef ds:uri="024f5ac7-e9d5-4ad8-8658-e9fe705846ee"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAA9CBFF-F379-4D9B-B674-AAE60B1F3E58}"/>
 </file>
</xml_diff>